<commit_message>
changes and new screen worked
SMS, Login, Bulk Upload
</commit_message>
<xml_diff>
--- a/uploads/downloadfiles/feesMasterBulkUpload.xlsx
+++ b/uploads/downloadfiles/feesMasterBulkUpload.xlsx
@@ -385,13 +385,13 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -427,15 +427,21 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"Tamil,English"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
-      <formula1>"New Student, Old Student, Vijayadashami,All"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>"Common, Standard Wise"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
+      <formula1>"2024-2025,2023-2024"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>"New Student, Old Student, Vijayadashami,All[NEW &amp; OLD]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"PRE.K.G,L.K.G,U.K.G,I,II,III,IV,V,VI,VII,VIII,IX,X,XI_Maths_Biology,XI_Maths_ComputerScience,XI_Biology_ComputerScience,XI_Commerce_ComputerScience,XI_All,XII_Maths_Biology,XII_Maths_ComputerScience,XII_Biology_ComputerScience,XII_Commerce_ComputerScience"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>